<commit_message>
calibration of Z/Pi matrix
</commit_message>
<xml_diff>
--- a/Data/Calibration/ConsumptionParameters/Grouping_CEX_cons_into_17groups.xlsx
+++ b/Data/Calibration/ConsumptionParameters/Grouping_CEX_cons_into_17groups.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>Category</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Shelter</t>
   </si>
   <si>
-    <t>SHELTER</t>
-  </si>
-  <si>
     <t>Level 3, "Shelter"</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>Level 3, "Public and other transportation"</t>
   </si>
   <si>
-    <t>New and used cares, fees, and maintenance</t>
-  </si>
-  <si>
     <t>VEHPURCH + VEHOTHXP</t>
   </si>
   <si>
@@ -202,16 +196,161 @@
   </si>
   <si>
     <t>HHFURNSH - MAJAPPL</t>
+  </si>
+  <si>
+    <t>PCE Line Number</t>
+  </si>
+  <si>
+    <t>239, 97</t>
+  </si>
+  <si>
+    <t>New and used cars, fees, and maintenance</t>
+  </si>
+  <si>
+    <t>187, 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Net expenditures abroad by U.S. residents</t>
+  </si>
+  <si>
+    <t>119, 168</t>
+  </si>
+  <si>
+    <t>161, 276, 280, 283</t>
+  </si>
+  <si>
+    <t>Not sure if postal service, line 280 should be here</t>
+  </si>
+  <si>
+    <t>246, 294</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Less: Expenditures in the United States by nonresidents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Final consumption expenditures of nonprofit institutions serving households (NPISH) </t>
+  </si>
+  <si>
+    <t>21 ex 28, 60 ex 61</t>
+  </si>
+  <si>
+    <t>102, 61</t>
+  </si>
+  <si>
+    <t>229, 72, 101</t>
+  </si>
+  <si>
+    <t>910050 (for homeowner), RNTDWELL for renter</t>
+  </si>
+  <si>
+    <t>PCE range of lines</t>
+  </si>
+  <si>
+    <t>36, 140, 124, 205, 328</t>
+  </si>
+  <si>
+    <t>97-100</t>
+  </si>
+  <si>
+    <t>111-117</t>
+  </si>
+  <si>
+    <t>143-147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">151-160, </t>
+  </si>
+  <si>
+    <t>4-20, 187-194</t>
+  </si>
+  <si>
+    <t>195-204</t>
+  </si>
+  <si>
+    <t>72-96, 101, 229-242</t>
+  </si>
+  <si>
+    <t>161-167, 276-283</t>
+  </si>
+  <si>
+    <t>284-291</t>
+  </si>
+  <si>
+    <t>246-273, 294-297</t>
+  </si>
+  <si>
+    <t>135-138, 298-320</t>
+  </si>
+  <si>
+    <t>135, 301, 298-300, 309</t>
+  </si>
+  <si>
+    <t>129, 321, 293</t>
+  </si>
+  <si>
+    <t>129-134, 293, 321-326</t>
+  </si>
+  <si>
+    <t>36-59, 124-128, 140-142, 205-227, 243-245, 327-335</t>
+  </si>
+  <si>
+    <t>Make sure to net foreign travel?</t>
+  </si>
+  <si>
+    <t>336-362</t>
+  </si>
+  <si>
+    <t>332-335</t>
+  </si>
+  <si>
+    <t>Need to net these out from non-durable total?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61-63, 102-110, </t>
+  </si>
+  <si>
+    <t>21-27, 29-35, 60, 67-69</t>
+  </si>
+  <si>
+    <t>64-66, 119-123, 168-185</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -234,14 +373,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -571,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D18"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -584,7 +737,7 @@
     <col min="4" max="4" width="64" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,8 +753,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -614,8 +773,14 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -628,8 +793,14 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -642,8 +813,14 @@
       <c r="E4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>139</v>
+      </c>
+      <c r="G4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -656,8 +833,17 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
@@ -665,199 +851,326 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>151</v>
+      </c>
+      <c r="G6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>28</v>
+      </c>
+      <c r="G8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>29</v>
       </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <v>195</v>
+      </c>
+      <c r="G10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
         <v>50</v>
       </c>
-      <c r="C16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <v>111</v>
+      </c>
+      <c r="G16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
         <v>56</v>
       </c>
-      <c r="C18" t="s">
+      <c r="F18">
+        <v>284</v>
+      </c>
+      <c r="G18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20">
+        <v>143</v>
+      </c>
+      <c r="G20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21">
+        <v>332</v>
+      </c>
+      <c r="G21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22">
+        <v>336</v>
+      </c>
+      <c r="G22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" t="s">
         <v>57</v>
-      </c>
-      <c r="E18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>